<commit_message>
* Reward 지급 방식 수정. (group)  * Inventory 저장 기능 준비.
</commit_message>
<xml_diff>
--- a/input/Domains/Game/ItemTable.xlsx
+++ b/input/Domains/Game/ItemTable.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="ITEM" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="EQUIP" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="CARD" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -424,17 +425,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>itemId</t>
+          <t>equipId</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>itemNameId</t>
+          <t>nameId</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>itemDescId</t>
+          <t>descId</t>
         </is>
       </c>
     </row>
@@ -465,17 +466,94 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>아이템 ID (정본)</t>
+          <t>장비 ID (정본)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>아이템 이름 텍스트 ID</t>
+          <t>이름 텍스트 ID</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>아이템 설명 텍스트 ID</t>
+          <t>설명 텍스트 ID</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>cardId</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nameId</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>descId</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>pk</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>카드 ID (정본)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>이름 텍스트 ID</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>설명 텍스트 ID</t>
         </is>
       </c>
     </row>

</xml_diff>